<commit_message>
23_1. Firefox added + Parallel
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t xml:space="preserve">testname</t>
   </si>
   <si>
     <t xml:space="preserve">execute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">browser</t>
   </si>
   <si>
     <t xml:space="preserve">username</t>
@@ -44,6 +47,9 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
@@ -54,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firefox</t>
   </si>
   <si>
     <t xml:space="preserve">somewho</t>
@@ -225,11 +234,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -247,7 +256,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -271,21 +282,23 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -309,21 +322,23 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -347,21 +362,23 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -385,21 +402,23 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -423,21 +442,23 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -28337,27 +28358,27 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -28383,19 +28404,19 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -28421,19 +28442,19 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -28459,19 +28480,19 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>

</xml_diff>

<commit_message>
25_0. Added PageFactory like bad example of usage
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
   <si>
     <t xml:space="preserve">testname</t>
   </si>
@@ -83,6 +83,12 @@
     <t xml:space="preserve">somehow</t>
   </si>
   <si>
+    <t xml:space="preserve">testAmazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'</t>
+  </si>
+  <si>
     <t xml:space="preserve">testdescription</t>
   </si>
   <si>
@@ -108,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
   </si>
 </sst>
 </file>
@@ -234,11 +243,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -481,12 +490,24 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -509,12 +530,24 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -28358,27 +28391,27 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -28407,16 +28440,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -28445,16 +28478,16 @@
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -28478,21 +28511,21 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -28516,12 +28549,22 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>

</xml_diff>

<commit_message>
25_1. Get menutext from XLSX doc
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
   <si>
     <t xml:space="preserve">testname</t>
   </si>
@@ -41,6 +41,9 @@
     <t xml:space="preserve">fname</t>
   </si>
   <si>
+    <t xml:space="preserve">menutext</t>
+  </si>
+  <si>
     <t xml:space="preserve">loginTest0</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve">someone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'</t>
   </si>
   <si>
     <t xml:space="preserve">no</t>
@@ -86,7 +92,10 @@
     <t xml:space="preserve">testAmazon</t>
   </si>
   <si>
-    <t xml:space="preserve">'</t>
+    <t xml:space="preserve">Computer Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computers &amp; Tablets</t>
   </si>
   <si>
     <t xml:space="preserve">testdescription</t>
@@ -243,8 +252,8 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -268,7 +277,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -291,24 +302,26 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -331,24 +344,26 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -371,24 +386,26 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -411,24 +428,26 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -451,24 +470,26 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -491,24 +512,26 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -531,24 +554,26 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -28391,7 +28416,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -28402,16 +28427,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -28437,19 +28462,19 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -28475,19 +28500,19 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -28513,19 +28538,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -28551,19 +28576,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>

</xml_diff>